<commit_message>
Added Sprint 5 files and updated all existing Drive documents to their latest versions. Included all submissions within the scope of BIL495. (thanks to the team)
</commit_message>
<xml_diff>
--- a/Sprint_2/Requirement_ID-Table_v1.xlsx
+++ b/Sprint_2/Requirement_ID-Table_v1.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
   <si>
     <t>Requirement ID</t>
   </si>
@@ -40,7 +40,7 @@
     <t>FR-H03</t>
   </si>
   <si>
-    <t>The system shall allow the user to view the suggested destinations and remove unwanted stops, after which the system shall automatically regenerate the optimized route.</t>
+    <t>The system shall allow the user to view the suggested destinations and remove unwanted stops or add new stops, after which the system shall automatically regenerate the optimized route.</t>
   </si>
   <si>
     <t>FR-H04</t>
@@ -67,6 +67,30 @@
     <t>The system shall estimate the average visiting duration for each stop, use these estimations when planning time-limited trips, and display them to the user.</t>
   </si>
   <si>
+    <t>FR-L08</t>
+  </si>
+  <si>
+    <t>The system shall automatically regenerate the optimized route when a user removes or adds a destination within the itinerary view.</t>
+  </si>
+  <si>
+    <t>FR-L09</t>
+  </si>
+  <si>
+    <t>The user shall be able to repeatedly modify the itinerary (e.g., remove or add POIs), and the system shall automatically regenerate the optimized route accordingly.</t>
+  </si>
+  <si>
+    <t>FR-L10</t>
+  </si>
+  <si>
+    <t>The system shall provide route-generation and recommendation support for at least twenty (20) cities or regions across Türkiye.</t>
+  </si>
+  <si>
+    <t>FR-L11</t>
+  </si>
+  <si>
+    <t>The system shall present a brief summary including total estimated distance and duration once a new route is generated.</t>
+  </si>
+  <si>
     <t>EIR-H01</t>
   </si>
   <si>
@@ -76,6 +100,30 @@
     <t>The system shall operate through a web-based user interface, accessible from both: desktop browsers, mobile browsers.</t>
   </si>
   <si>
+    <t>EIR-L02</t>
+  </si>
+  <si>
+    <t>The system shall allow the user to click on pins (markers) displayed on the map to open a detailed information page for the selected Point of Interest (POI).</t>
+  </si>
+  <si>
+    <t>EIR-L03</t>
+  </si>
+  <si>
+    <t>The system shall communicate with OpenStreetMap layers through standardized API requests compatible with OSRM data format</t>
+  </si>
+  <si>
+    <t>EIR-L04</t>
+  </si>
+  <si>
+    <t>The system shall maintain bidirectional navigation between the map interface and POI detail page, allowing the user to return to the map view with one action.</t>
+  </si>
+  <si>
+    <t>EIR-L05</t>
+  </si>
+  <si>
+    <t>The system shall validate user inputs and display a clear error message without performing route calculation.</t>
+  </si>
+  <si>
     <t>PR-H01</t>
   </si>
   <si>
@@ -89,13 +137,25 @@
   </si>
   <si>
     <t>The system shall support at least 1000 users.</t>
+  </si>
+  <si>
+    <t>PR-L03</t>
+  </si>
+  <si>
+    <t>The system shall start audio playback within 2 seconds after the user requests TTS for a POI description.</t>
+  </si>
+  <si>
+    <t>PR-L04</t>
+  </si>
+  <si>
+    <t>The system shall cache static POI and media data locally to minimize repeated API calls and improve response time.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -113,8 +173,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -143,12 +207,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFF4CCCC"/>
         <bgColor rgb="FFF4CCCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -185,6 +243,9 @@
     <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -196,9 +257,6 @@
     </xf>
     <xf borderId="1" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -268,7 +326,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:C11" displayName="Table_1" name="Table_1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:C21" displayName="Table_1" name="Table_1" id="1">
   <tableColumns count="3">
     <tableColumn name="Requirement ID" id="1"/>
     <tableColumn name="Requirement Type" id="2"/>
@@ -484,7 +542,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="13.38"/>
     <col customWidth="1" min="2" max="2" width="17.13"/>
-    <col customWidth="1" min="3" max="3" width="139.13"/>
+    <col customWidth="1" min="3" max="3" width="142.88"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -576,43 +634,370 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="4"/>
+      <c r="V9" s="4"/>
+      <c r="W9" s="4"/>
+      <c r="X9" s="4"/>
+      <c r="Y9" s="4"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="6" t="s">
+      <c r="B10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4"/>
+      <c r="S10" s="4"/>
+      <c r="T10" s="4"/>
+      <c r="U10" s="4"/>
+      <c r="V10" s="4"/>
+      <c r="W10" s="4"/>
+      <c r="X10" s="4"/>
+      <c r="Y10" s="4"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="B11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="6" t="s">
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4"/>
+      <c r="S11" s="4"/>
+      <c r="T11" s="4"/>
+      <c r="U11" s="4"/>
+      <c r="V11" s="4"/>
+      <c r="W11" s="4"/>
+      <c r="X11" s="4"/>
+      <c r="Y11" s="4"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="7" t="s">
+      <c r="B12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="4"/>
+      <c r="U12" s="4"/>
+      <c r="V12" s="4"/>
+      <c r="W12" s="4"/>
+      <c r="X12" s="4"/>
+      <c r="Y12" s="4"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="14">
-      <c r="C14" s="8"/>
+      <c r="A14" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4"/>
+      <c r="S14" s="4"/>
+      <c r="T14" s="4"/>
+      <c r="U14" s="4"/>
+      <c r="V14" s="4"/>
+      <c r="W14" s="4"/>
+      <c r="X14" s="4"/>
+      <c r="Y14" s="4"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="4"/>
+      <c r="S15" s="4"/>
+      <c r="T15" s="4"/>
+      <c r="U15" s="4"/>
+      <c r="V15" s="4"/>
+      <c r="W15" s="4"/>
+      <c r="X15" s="4"/>
+      <c r="Y15" s="4"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="4"/>
+      <c r="R16" s="4"/>
+      <c r="S16" s="4"/>
+      <c r="T16" s="4"/>
+      <c r="U16" s="4"/>
+      <c r="V16" s="4"/>
+      <c r="W16" s="4"/>
+      <c r="X16" s="4"/>
+      <c r="Y16" s="4"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="4"/>
+      <c r="S17" s="4"/>
+      <c r="T17" s="4"/>
+      <c r="U17" s="4"/>
+      <c r="V17" s="4"/>
+      <c r="W17" s="4"/>
+      <c r="X17" s="4"/>
+      <c r="Y17" s="4"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="4"/>
+      <c r="R20" s="4"/>
+      <c r="S20" s="4"/>
+      <c r="T20" s="4"/>
+      <c r="U20" s="4"/>
+      <c r="V20" s="4"/>
+      <c r="W20" s="4"/>
+      <c r="X20" s="4"/>
+      <c r="Y20" s="4"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4"/>
+      <c r="R21" s="4"/>
+      <c r="S21" s="4"/>
+      <c r="T21" s="4"/>
+      <c r="U21" s="4"/>
+      <c r="V21" s="4"/>
+      <c r="W21" s="4"/>
+      <c r="X21" s="4"/>
+      <c r="Y21" s="4"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:C1 C14">
+  <conditionalFormatting sqref="A1:C1">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>

</xml_diff>